<commit_message>
added STM32L051, STM32F401CC, STM32F103C8, GD32F303CC
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\__my_github\dhrystone_score\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A67CC03A-FE42-49C9-9C39-3B9C12998795}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2016" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2952" yWindow="-108" windowWidth="22080" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -18,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$H$39</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
   <si>
     <t>MCU</t>
   </si>
@@ -147,17 +146,33 @@
   </si>
   <si>
     <t>BCM2835(RPi Zero)</t>
+  </si>
+  <si>
+    <t>STM32L051C8T6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Os</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>STM32L051C8T6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>O3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -165,7 +180,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -173,7 +188,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -182,7 +197,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -191,7 +206,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -200,7 +215,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -208,7 +223,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -216,7 +231,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -224,7 +239,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -232,7 +247,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -241,7 +256,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -250,7 +265,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -258,7 +273,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -267,7 +282,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -275,7 +290,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -284,7 +299,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -293,7 +308,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -301,14 +316,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1110,14 +1125,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -1130,7 +1145,7 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1178,7 +1193,7 @@
         <v>5.5914329853057705</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1203,7 +1218,7 @@
         <v>2.6167906371231004</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1228,7 +1243,7 @@
         <v>2.1624314725466349</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -1253,7 +1268,7 @@
         <v>1.0416397576395944</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1278,7 +1293,7 @@
         <v>1.1549349910192255</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1318,7 @@
         <v>1.1292697689965761</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1328,7 +1343,7 @@
         <v>1.3080344814632157</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1353,7 +1368,7 @@
         <v>1.1562489102354021</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1378,7 +1393,7 @@
         <v>1.2580724216937982</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1403,7 +1418,7 @@
         <v>1.1531565839498223</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1428,7 +1443,7 @@
         <v>0.69996060061771248</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1453,7 +1468,7 @@
         <v>1.3005026130478805</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1478,7 +1493,7 @@
         <v>1.1151096465013213</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1503,7 +1518,7 @@
         <v>0.58482528110796794</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1528,7 +1543,7 @@
         <v>0.90756468231642151</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1553,7 +1568,7 @@
         <v>0.73728167725565363</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +1593,7 @@
         <v>0.58314750366216639</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>0.7957941325143657</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1628,34 +1643,34 @@
         <v>0.43125413982411531</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2">
-        <v>27</v>
-      </c>
-      <c r="F21" s="3">
+        <v>25.3</v>
+      </c>
+      <c r="F21" s="2">
         <f>1000/E21/1.757</f>
-        <v>21.079702354602755</v>
+        <v>22.496125042461436</v>
       </c>
       <c r="G21" s="2">
         <f>F21/D21</f>
-        <v>1.3174813971626722</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>0.70300390757691988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -1667,123 +1682,123 @@
         <v>16</v>
       </c>
       <c r="E22" s="2">
-        <v>27.23</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3">
         <f>1000/E22/1.757</f>
-        <v>20.901651251350508</v>
+        <v>21.079702354602755</v>
       </c>
       <c r="G22" s="2">
         <f>F22/D22</f>
-        <v>1.3063532032094067</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>1.3174813971626722</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="1">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2">
-        <v>27.52</v>
+        <v>27.23</v>
       </c>
       <c r="F23" s="3">
         <f>1000/E23/1.757</f>
-        <v>20.681394025227995</v>
+        <v>20.901651251350508</v>
       </c>
       <c r="G23" s="2">
         <f>F23/D23</f>
-        <v>0.43086237552558321</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>1.3063532032094067</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="1">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E24" s="2">
-        <v>55.1</v>
+        <v>27.52</v>
       </c>
       <c r="F24" s="3">
         <f>1000/E24/1.757</f>
-        <v>10.329436725485923</v>
+        <v>20.681394025227995</v>
       </c>
       <c r="G24" s="2">
         <f>F24/D24</f>
-        <v>1.2911795906857404</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>0.43086237552558321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E25" s="2">
-        <v>59</v>
-      </c>
-      <c r="F25" s="3">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F25" s="2">
         <f>1000/E25/1.757</f>
-        <v>9.64664345041143</v>
+        <v>15.466085966692239</v>
       </c>
       <c r="G25" s="2">
         <f>F25/D25</f>
-        <v>1.2058304313014288</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>0.96663037291826492</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="1">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2">
-        <v>61.5</v>
-      </c>
-      <c r="F26" s="3">
+        <v>42.9</v>
+      </c>
+      <c r="F26" s="2">
         <f>1000/E26/1.757</f>
-        <v>9.2545034727524289</v>
+        <v>13.266945537861874</v>
       </c>
       <c r="G26" s="2">
         <f>F26/D26</f>
-        <v>1.1568129340940536</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>0.41459204805818356</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>25</v>
@@ -1792,70 +1807,70 @@
         <v>8</v>
       </c>
       <c r="E27" s="2">
-        <v>61.55</v>
+        <v>55.1</v>
       </c>
       <c r="F27" s="3">
         <f>1000/E27/1.757</f>
-        <v>9.2469855982822793</v>
+        <v>10.329436725485923</v>
       </c>
       <c r="G27" s="2">
         <f>F27/D27</f>
-        <v>1.1558731997852849</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>1.2911795906857404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E28" s="2">
-        <v>71.900000000000006</v>
+        <v>59</v>
       </c>
       <c r="F28" s="3">
         <f>1000/E28/1.757</f>
-        <v>7.9158826644544416</v>
+        <v>9.64664345041143</v>
       </c>
       <c r="G28" s="2">
         <f>F28/D28</f>
-        <v>0.4947426665284026</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>1.2058304313014288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E29" s="2">
-        <v>74</v>
+        <v>61.5</v>
       </c>
       <c r="F29" s="3">
         <f>1000/E29/1.757</f>
-        <v>7.691242751003708</v>
+        <v>9.2545034727524289</v>
       </c>
       <c r="G29" s="2">
         <f>F29/D29</f>
-        <v>0.48070267193773175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>1.1568129340940536</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -1867,221 +1882,321 @@
         <v>8</v>
       </c>
       <c r="E30" s="2">
-        <v>80</v>
+        <v>61.55</v>
       </c>
       <c r="F30" s="3">
         <f>1000/E30/1.757</f>
-        <v>7.1143995446784292</v>
+        <v>9.2469855982822793</v>
       </c>
       <c r="G30" s="2">
         <f>F30/D30</f>
-        <v>0.88929994308480365</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>1.1558731997852849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E31" s="2">
-        <v>96</v>
-      </c>
-      <c r="F31" s="3">
+        <v>62.1</v>
+      </c>
+      <c r="F31" s="2">
         <f>1000/E31/1.757</f>
-        <v>5.9286662872320246</v>
+        <v>9.1650879802620668</v>
       </c>
       <c r="G31" s="2">
         <f>F31/D31</f>
-        <v>0.74108328590400308</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>0.57281799876637918</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D32" s="1">
         <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>107.1</v>
+        <v>71.900000000000006</v>
       </c>
       <c r="F32" s="3">
         <f>1000/E32/1.757</f>
-        <v>5.314210677630947</v>
+        <v>7.9158826644544416</v>
       </c>
       <c r="G32" s="2">
         <f>F32/D32</f>
-        <v>0.33213816735193419</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>0.4947426665284026</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D33" s="1">
         <v>16</v>
       </c>
       <c r="E33" s="2">
-        <v>107.2</v>
+        <v>74</v>
       </c>
       <c r="F33" s="3">
         <f>1000/E33/1.757</f>
-        <v>5.3092533915510671</v>
+        <v>7.691242751003708</v>
       </c>
       <c r="G33" s="2">
         <f>F33/D33</f>
-        <v>0.3318283369719417</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>0.48070267193773175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E34" s="2">
-        <v>108.1</v>
+        <v>80</v>
       </c>
       <c r="F34" s="3">
         <f>1000/E34/1.757</f>
-        <v>5.265050541852677</v>
+        <v>7.1143995446784292</v>
       </c>
       <c r="G34" s="2">
         <f>F34/D34</f>
-        <v>0.32906565886579231</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>0.88929994308480365</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D35" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E35" s="2">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="F35" s="3">
         <f>1000/E35/1.757</f>
-        <v>4.7037352361510276</v>
+        <v>5.9286662872320246</v>
       </c>
       <c r="G35" s="2">
         <f>F35/D35</f>
-        <v>0.29398345225943923</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>0.74108328590400308</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D36" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2">
-        <v>254</v>
-      </c>
-      <c r="F36" s="2">
+        <v>107.1</v>
+      </c>
+      <c r="F36" s="3">
         <f>1000/E36/1.757</f>
-        <v>2.2407557621034426</v>
+        <v>5.314210677630947</v>
       </c>
       <c r="G36" s="2">
         <f>F36/D36</f>
-        <v>9.3364823420976781E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>0.33213816735193419</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D37" s="1">
         <v>16</v>
       </c>
       <c r="E37" s="2">
-        <v>883</v>
+        <v>107.2</v>
       </c>
       <c r="F37" s="3">
         <f>1000/E37/1.757</f>
-        <v>0.64456621016339111</v>
+        <v>5.3092533915510671</v>
       </c>
       <c r="G37" s="2">
         <f>F37/D37</f>
-        <v>4.0285388135211944E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>0.3318283369719417</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D38" s="1">
         <v>16</v>
       </c>
       <c r="E38" s="2">
-        <v>884</v>
+        <v>108.1</v>
       </c>
       <c r="F38" s="3">
         <f>1000/E38/1.757</f>
-        <v>0.64383706286682618</v>
+        <v>5.265050541852677</v>
       </c>
       <c r="G38" s="2">
         <f>F38/D38</f>
+        <v>0.32906565886579231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="1">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2">
+        <v>121</v>
+      </c>
+      <c r="F39" s="3">
+        <f>1000/E39/1.757</f>
+        <v>4.7037352361510276</v>
+      </c>
+      <c r="G39" s="2">
+        <f>F39/D39</f>
+        <v>0.29398345225943923</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="1">
+        <v>24</v>
+      </c>
+      <c r="E40" s="2">
+        <v>254</v>
+      </c>
+      <c r="F40" s="2">
+        <f>1000/E40/1.757</f>
+        <v>2.2407557621034426</v>
+      </c>
+      <c r="G40" s="2">
+        <f>F40/D40</f>
+        <v>9.3364823420976781E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="1">
+        <v>16</v>
+      </c>
+      <c r="E41" s="2">
+        <v>883</v>
+      </c>
+      <c r="F41" s="3">
+        <f>1000/E41/1.757</f>
+        <v>0.64456621016339111</v>
+      </c>
+      <c r="G41" s="2">
+        <f>F41/D41</f>
+        <v>4.0285388135211944E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="1">
+        <v>16</v>
+      </c>
+      <c r="E42" s="2">
+        <v>884</v>
+      </c>
+      <c r="F42" s="3">
+        <f>1000/E42/1.757</f>
+        <v>0.64383706286682618</v>
+      </c>
+      <c r="G42" s="2">
+        <f>F42/D42</f>
         <v>4.0239816429176636E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H39" xr:uid="{621C4AF1-4861-43BF-8BF4-FCB17F273E29}"/>
-  <sortState ref="A2:H38">
-    <sortCondition descending="1" ref="F2:F38"/>
+  <autoFilter ref="A1:H39"/>
+  <sortState ref="A2:G43">
+    <sortCondition descending="1" ref="F2:F43"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>